<commit_message>
CsvJsonReport Sessions can wrap over to next day. Handle encoding     - Store result in a file to handle encoding     - Cleanup among exmaple files.
commit f6c3f31a4a38a9f35dec36a6b13dd710faaeacb7
Author: Per Ekskog <per.ekskog@gmail.com>
Date:   Thu Nov 10 08:51:01 2016 +0100

    CsvJsonReport: wip - task starting next day
</commit_message>
<xml_diff>
--- a/CsvJsonReport/2column-short.xlsx
+++ b/CsvJsonReport/2column-short.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uabpan\tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/per/git-public/playground/CsvJsonReport/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14600"/>
   </bookViews>
   <sheets>
     <sheet name="Book1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Jobb 08</t>
   </si>
@@ -47,12 +53,27 @@
   </si>
   <si>
     <t>Annat 07</t>
+  </si>
+  <si>
+    <t>Slöläs</t>
+  </si>
+  <si>
+    <t>Jobb 09</t>
+  </si>
+  <si>
+    <t>Annat</t>
+  </si>
+  <si>
+    <t>Kaffe</t>
+  </si>
+  <si>
+    <t>Sova</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,23 +420,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -428,8 +452,14 @@
       <c r="D2" s="1">
         <v>0.3125</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -440,21 +470,33 @@
       <c r="D3" s="1">
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>0.35416666666666669</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>0.375</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -462,7 +504,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -476,7 +518,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -490,7 +532,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>0.375</v>
       </c>
@@ -498,12 +540,12 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -511,7 +553,7 @@
         <v>0.3125</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -519,9 +561,17 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
       <c r="B17" s="1">
-        <v>0.375</v>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>0.10416666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -535,7 +585,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -547,7 +597,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>